<commit_message>
Symbolic names to jaen
</commit_message>
<xml_diff>
--- a/pub-jaen/jaen/data_gen/openc2_genj.xlsx
+++ b/pub-jaen/jaen/data_gen/openc2_genj.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="478">
   <si>
-    <t>Generated from data\openc2.jaen, Fri Feb 24 14:29:42 2017</t>
+    <t>Generated from data\openc2.jaen, Sat Feb 25 10:40:32 2017</t>
   </si>
   <si>
     <t>module</t>
@@ -1224,7 +1224,7 @@
     <t>Value of the domain name</t>
   </si>
   <si>
-    <t>resolves-to (required)</t>
+    <t>resolves_to (optional)</t>
   </si>
   <si>
     <t>dnvalues (Array)</t>

</xml_diff>

<commit_message>
Update ipv4 in socket-addr
</commit_message>
<xml_diff>
--- a/pub-jaen/jaen/data_gen/openc2_genj.xlsx
+++ b/pub-jaen/jaen/data_gen/openc2_genj.xlsx
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="461">
-  <si>
-    <t>Generated from data\openc2.jaen, Mon Mar  6 16:41:56 2017</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="463">
+  <si>
+    <t>Generated from data\openc2.jaen, Fri Mar 10 08:20:43 2017</t>
   </si>
   <si>
     <t>module</t>
@@ -1288,6 +1288,12 @@
   </si>
   <si>
     <t>socket-addr</t>
+  </si>
+  <si>
+    <t>ipv4</t>
+  </si>
+  <si>
+    <t>ipv6</t>
   </si>
   <si>
     <t>mac</t>
@@ -5333,7 +5339,7 @@
         <v>1</v>
       </c>
       <c r="C379" s="8" t="s">
-        <v>365</v>
+        <v>424</v>
       </c>
       <c r="D379" s="8" t="s">
         <v>117</v>
@@ -5345,7 +5351,7 @@
         <v>2</v>
       </c>
       <c r="C380" s="8" t="s">
-        <v>366</v>
+        <v>425</v>
       </c>
       <c r="D380" s="8" t="s">
         <v>119</v>
@@ -5357,7 +5363,7 @@
         <v>3</v>
       </c>
       <c r="C381" s="8" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="D381" s="8" t="s">
         <v>121</v>
@@ -5369,7 +5375,7 @@
         <v>4</v>
       </c>
       <c r="C382" s="8" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D382" s="8" t="s">
         <v>109</v>
@@ -5381,7 +5387,7 @@
         <v>15</v>
       </c>
       <c r="B385" s="5" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="C385" s="5"/>
       <c r="D385" s="5"/>
@@ -5403,7 +5409,7 @@
         <v>92</v>
       </c>
       <c r="B387" s="6" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="C387" s="6"/>
       <c r="D387" s="6"/>
@@ -5428,13 +5434,13 @@
         <v>1</v>
       </c>
       <c r="C390" s="8" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="D390" s="8" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="E390" s="8" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
     </row>
     <row r="391" spans="1:5">
@@ -5442,13 +5448,13 @@
         <v>2</v>
       </c>
       <c r="C391" s="8" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="D391" s="8" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="E391" s="8" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
     </row>
     <row r="394" spans="1:5">
@@ -5564,7 +5570,7 @@
         <v>15</v>
       </c>
       <c r="B412" s="5" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="C412" s="5"/>
       <c r="D412" s="5"/>
@@ -5600,7 +5606,7 @@
         <v>15</v>
       </c>
       <c r="B418" s="5" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="C418" s="5"/>
       <c r="D418" s="5"/>
@@ -5636,7 +5642,7 @@
         <v>15</v>
       </c>
       <c r="B424" s="5" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="C424" s="5"/>
       <c r="D424" s="5"/>
@@ -6704,7 +6710,7 @@
         <v>55</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="C120" s="5"/>
       <c r="D120" s="5"/>
@@ -6714,7 +6720,7 @@
         <v>92</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="C121" s="6"/>
       <c r="D121" s="6"/>
@@ -6735,10 +6741,10 @@
         <v>1</v>
       </c>
       <c r="C124" s="8" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -6746,10 +6752,10 @@
         <v>6</v>
       </c>
       <c r="C125" s="8" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -6757,10 +6763,10 @@
         <v>17</v>
       </c>
       <c r="C126" s="8" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -6768,7 +6774,7 @@
         <v>55</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C128" s="5"/>
       <c r="D128" s="5"/>
@@ -6778,7 +6784,7 @@
         <v>92</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="C129" s="6"/>
       <c r="D129" s="6"/>
@@ -6799,10 +6805,10 @@
         <v>20</v>
       </c>
       <c r="C132" s="8" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="D132" s="8" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -6810,10 +6816,10 @@
         <v>21</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -6821,10 +6827,10 @@
         <v>22</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -6832,10 +6838,10 @@
         <v>23</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -6843,10 +6849,10 @@
         <v>25</v>
       </c>
       <c r="C136" s="8" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -6854,10 +6860,10 @@
         <v>80</v>
       </c>
       <c r="C137" s="8" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -6865,10 +6871,10 @@
         <v>443</v>
       </c>
       <c r="C138" s="8" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use ip-addr in domain-name and ip-connection
</commit_message>
<xml_diff>
--- a/pub-jaen/jaen/data_gen/openc2_genj.xlsx
+++ b/pub-jaen/jaen/data_gen/openc2_genj.xlsx
@@ -16,9 +16,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="463">
-  <si>
-    <t>Generated from data\openc2.jaen, Fri Mar 10 08:20:43 2017</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="462">
+  <si>
+    <t>Generated from data\openc2.jaen, Fri Mar 10 13:38:29 2017</t>
   </si>
   <si>
     <t>module</t>
@@ -1098,25 +1098,25 @@
     <t>resolves_to (optional)</t>
   </si>
   <si>
-    <t>dnvalues (Array)</t>
+    <t>ip-addrs (Array)</t>
   </si>
   <si>
     <t>List of IP addresses or domain names</t>
   </si>
   <si>
-    <t>dnvalues</t>
-  </si>
-  <si>
-    <t>dnvalue (Choice)</t>
-  </si>
-  <si>
-    <t>dnvalue</t>
-  </si>
-  <si>
-    <t>v4</t>
-  </si>
-  <si>
-    <t>v6</t>
+    <t>ip-addrs</t>
+  </si>
+  <si>
+    <t>ip-addr (Choice)</t>
+  </si>
+  <si>
+    <t>ip-addr</t>
+  </si>
+  <si>
+    <t>ipv4</t>
+  </si>
+  <si>
+    <t>ipv6</t>
   </si>
   <si>
     <t>name</t>
@@ -1146,10 +1146,19 @@
     <t>TODO: finish</t>
   </si>
   <si>
+    <t>ipv4-str</t>
+  </si>
+  <si>
+    <t>IPv4 address or range in CIDR notation</t>
+  </si>
+  <si>
     <t>ipv4-addr</t>
   </si>
   <si>
-    <t>Specifies one or more IPv4 addresses using CIDR notation</t>
+    <t>ipv4-str (String)</t>
+  </si>
+  <si>
+    <t>Specifies one or more IPv4 addresses</t>
   </si>
   <si>
     <t>resolves_to_refs (optional)</t>
@@ -1170,10 +1179,19 @@
     <t>Specifies a reference to one or more autonomous systems (AS) that the IPv4 address belongs to.</t>
   </si>
   <si>
+    <t>ipv6-str</t>
+  </si>
+  <si>
+    <t>IPv6 address or range</t>
+  </si>
+  <si>
     <t>ipv6-addr</t>
   </si>
   <si>
-    <t>ipv4-str</t>
+    <t>ipv6-str (String)</t>
+  </si>
+  <si>
+    <t>Specifies one or more IPv6 addresses</t>
   </si>
   <si>
     <t>mac-addrs</t>
@@ -1209,9 +1227,6 @@
     <t>src_addr (optional)</t>
   </si>
   <si>
-    <t>socket-addr (Choice)</t>
-  </si>
-  <si>
     <t>source address</t>
   </si>
   <si>
@@ -1282,24 +1297,6 @@
   </si>
   <si>
     <t>0x8847 Multi-Protocol Label Switching</t>
-  </si>
-  <si>
-    <t>socket-addrs</t>
-  </si>
-  <si>
-    <t>socket-addr</t>
-  </si>
-  <si>
-    <t>ipv4</t>
-  </si>
-  <si>
-    <t>ipv6</t>
-  </si>
-  <si>
-    <t>mac</t>
-  </si>
-  <si>
-    <t>dns</t>
   </si>
   <si>
     <t>port</t>
@@ -1888,7 +1885,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E427"/>
+  <dimension ref="A2:E422"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4831,216 +4828,218 @@
         <v>16</v>
       </c>
       <c r="B316" s="6" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C316" s="6"/>
       <c r="D316" s="6"/>
       <c r="E316" s="6"/>
     </row>
-    <row r="318" spans="1:5">
-      <c r="B318" s="7" t="s">
+    <row r="317" spans="1:5">
+      <c r="A317" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B317" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="C317" s="6"/>
+      <c r="D317" s="6"/>
+      <c r="E317" s="6"/>
+    </row>
+    <row r="320" spans="1:5">
+      <c r="A320" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B320" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="C320" s="5"/>
+      <c r="D320" s="5"/>
+      <c r="E320" s="5"/>
+    </row>
+    <row r="321" spans="1:5">
+      <c r="A321" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B321" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C321" s="6"/>
+      <c r="D321" s="6"/>
+      <c r="E321" s="6"/>
+    </row>
+    <row r="323" spans="1:5">
+      <c r="B323" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C318" s="7" t="s">
+      <c r="C323" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D318" s="7" t="s">
+      <c r="D323" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E318" s="7" t="s">
+      <c r="E323" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="319" spans="1:5">
-      <c r="B319" s="8">
+    <row r="324" spans="1:5">
+      <c r="B324" s="8">
         <v>1</v>
       </c>
-      <c r="C319" s="8" t="s">
+      <c r="C324" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="D319" s="8" t="s">
+      <c r="D324" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="E324" s="8" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5">
+      <c r="B325" s="8">
+        <v>2</v>
+      </c>
+      <c r="C325" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="D325" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="E325" s="8" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5">
+      <c r="B326" s="8">
+        <v>3</v>
+      </c>
+      <c r="C326" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="D326" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="E326" s="8" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5">
+      <c r="A329" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B329" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="C329" s="5"/>
+      <c r="D329" s="5"/>
+      <c r="E329" s="5"/>
+    </row>
+    <row r="330" spans="1:5">
+      <c r="A330" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B330" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E319" s="8" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="320" spans="1:5">
-      <c r="B320" s="8">
-        <v>2</v>
-      </c>
-      <c r="C320" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="D320" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="E320" s="8" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="321" spans="1:5">
-      <c r="B321" s="8">
-        <v>3</v>
-      </c>
-      <c r="C321" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="D321" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="E321" s="8" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="324" spans="1:5">
-      <c r="A324" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B324" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="C324" s="5"/>
-      <c r="D324" s="5"/>
-      <c r="E324" s="5"/>
-    </row>
-    <row r="325" spans="1:5">
-      <c r="A325" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B325" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C325" s="6"/>
-      <c r="D325" s="6"/>
-      <c r="E325" s="6"/>
-    </row>
-    <row r="327" spans="1:5">
-      <c r="B327" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C327" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D327" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E327" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="328" spans="1:5">
-      <c r="B328" s="8">
-        <v>1</v>
-      </c>
-      <c r="C328" s="8" t="s">
-        <v>357</v>
-      </c>
-      <c r="D328" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="E328" s="8" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="329" spans="1:5">
-      <c r="B329" s="8">
-        <v>2</v>
-      </c>
-      <c r="C329" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="D329" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="E329" s="8" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="330" spans="1:5">
-      <c r="B330" s="8">
-        <v>3</v>
-      </c>
-      <c r="C330" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="D330" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="E330" s="8" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="333" spans="1:5">
-      <c r="A333" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B333" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="C333" s="5"/>
-      <c r="D333" s="5"/>
-      <c r="E333" s="5"/>
+      <c r="C330" s="6"/>
+      <c r="D330" s="6"/>
+      <c r="E330" s="6"/>
+    </row>
+    <row r="331" spans="1:5">
+      <c r="A331" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B331" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="C331" s="6"/>
+      <c r="D331" s="6"/>
+      <c r="E331" s="6"/>
     </row>
     <row r="334" spans="1:5">
       <c r="A334" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B334" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="C334" s="5"/>
+      <c r="D334" s="5"/>
+      <c r="E334" s="5"/>
+    </row>
+    <row r="335" spans="1:5">
+      <c r="A335" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B334" s="6" t="s">
-        <v>351</v>
-      </c>
-      <c r="C334" s="6"/>
-      <c r="D334" s="6"/>
-      <c r="E334" s="6"/>
-    </row>
-    <row r="335" spans="1:5">
-      <c r="B335" s="8">
-        <v>0</v>
-      </c>
-      <c r="C335" s="8"/>
-      <c r="D335" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="E335" s="8"/>
+      <c r="B335" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C335" s="6"/>
+      <c r="D335" s="6"/>
+      <c r="E335" s="6"/>
+    </row>
+    <row r="337" spans="1:5">
+      <c r="B337" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C337" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D337" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E337" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="338" spans="1:5">
-      <c r="A338" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B338" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="C338" s="5"/>
-      <c r="D338" s="5"/>
-      <c r="E338" s="5"/>
+      <c r="B338" s="8">
+        <v>1</v>
+      </c>
+      <c r="C338" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="D338" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="E338" s="8" t="s">
+        <v>391</v>
+      </c>
     </row>
     <row r="339" spans="1:5">
-      <c r="A339" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B339" s="6" t="s">
-        <v>351</v>
-      </c>
-      <c r="C339" s="6"/>
-      <c r="D339" s="6"/>
-      <c r="E339" s="6"/>
+      <c r="B339" s="8">
+        <v>2</v>
+      </c>
+      <c r="C339" s="8" t="s">
+        <v>381</v>
+      </c>
+      <c r="D339" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="E339" s="8" t="s">
+        <v>383</v>
+      </c>
     </row>
     <row r="340" spans="1:5">
       <c r="B340" s="8">
-        <v>0</v>
-      </c>
-      <c r="C340" s="8"/>
+        <v>3</v>
+      </c>
+      <c r="C340" s="8" t="s">
+        <v>384</v>
+      </c>
       <c r="D340" s="8" t="s">
-        <v>388</v>
-      </c>
-      <c r="E340" s="8"/>
+        <v>385</v>
+      </c>
+      <c r="E340" s="8" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="343" spans="1:5">
       <c r="A343" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B343" s="5" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C343" s="5"/>
       <c r="D343" s="5"/>
@@ -5051,630 +5050,578 @@
         <v>16</v>
       </c>
       <c r="B344" s="6" t="s">
-        <v>29</v>
+        <v>351</v>
       </c>
       <c r="C344" s="6"/>
       <c r="D344" s="6"/>
       <c r="E344" s="6"/>
     </row>
-    <row r="346" spans="1:5">
-      <c r="B346" s="7" t="s">
+    <row r="345" spans="1:5">
+      <c r="B345" s="8">
+        <v>0</v>
+      </c>
+      <c r="C345" s="8"/>
+      <c r="D345" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E345" s="8"/>
+    </row>
+    <row r="348" spans="1:5">
+      <c r="A348" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B348" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="C348" s="5"/>
+      <c r="D348" s="5"/>
+      <c r="E348" s="5"/>
+    </row>
+    <row r="349" spans="1:5">
+      <c r="A349" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B349" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="C349" s="6"/>
+      <c r="D349" s="6"/>
+      <c r="E349" s="6"/>
+    </row>
+    <row r="350" spans="1:5">
+      <c r="B350" s="8">
+        <v>0</v>
+      </c>
+      <c r="C350" s="8"/>
+      <c r="D350" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="E350" s="8"/>
+    </row>
+    <row r="353" spans="1:5">
+      <c r="A353" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B353" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="C353" s="5"/>
+      <c r="D353" s="5"/>
+      <c r="E353" s="5"/>
+    </row>
+    <row r="354" spans="1:5">
+      <c r="A354" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B354" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C354" s="6"/>
+      <c r="D354" s="6"/>
+      <c r="E354" s="6"/>
+    </row>
+    <row r="356" spans="1:5">
+      <c r="B356" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C346" s="7" t="s">
+      <c r="C356" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D346" s="7" t="s">
+      <c r="D356" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E346" s="7" t="s">
+      <c r="E356" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="347" spans="1:5">
-      <c r="B347" s="8">
+    <row r="357" spans="1:5">
+      <c r="B357" s="8">
         <v>1</v>
       </c>
-      <c r="C347" s="8" t="s">
+      <c r="C357" s="8" t="s">
         <v>357</v>
       </c>
-      <c r="D347" s="8" t="s">
+      <c r="D357" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E347" s="8" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="350" spans="1:5">
-      <c r="A350" s="4" t="s">
+      <c r="E357" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="360" spans="1:5">
+      <c r="A360" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B350" s="5" t="s">
-        <v>391</v>
-      </c>
-      <c r="C350" s="5"/>
-      <c r="D350" s="5"/>
-      <c r="E350" s="5"/>
-    </row>
-    <row r="351" spans="1:5">
-      <c r="A351" s="4" t="s">
+      <c r="B360" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="C360" s="5"/>
+      <c r="D360" s="5"/>
+      <c r="E360" s="5"/>
+    </row>
+    <row r="361" spans="1:5">
+      <c r="A361" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B351" s="6" t="s">
+      <c r="B361" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C351" s="6"/>
-      <c r="D351" s="6"/>
-      <c r="E351" s="6"/>
-    </row>
-    <row r="353" spans="1:5">
-      <c r="B353" s="7" t="s">
+      <c r="C361" s="6"/>
+      <c r="D361" s="6"/>
+      <c r="E361" s="6"/>
+    </row>
+    <row r="363" spans="1:5">
+      <c r="B363" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C353" s="7" t="s">
+      <c r="C363" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D353" s="7" t="s">
+      <c r="D363" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E353" s="7" t="s">
+      <c r="E363" s="7" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="354" spans="1:5">
-      <c r="B354" s="8">
-        <v>1</v>
-      </c>
-      <c r="C354" s="8" t="s">
-        <v>392</v>
-      </c>
-      <c r="D354" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E354" s="8" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="357" spans="1:5">
-      <c r="A357" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B357" s="5" t="s">
-        <v>394</v>
-      </c>
-      <c r="C357" s="5"/>
-      <c r="D357" s="5"/>
-      <c r="E357" s="5"/>
-    </row>
-    <row r="358" spans="1:5">
-      <c r="A358" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B358" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C358" s="6"/>
-      <c r="D358" s="6"/>
-      <c r="E358" s="6"/>
-    </row>
-    <row r="359" spans="1:5">
-      <c r="A359" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B359" s="6" t="s">
-        <v>395</v>
-      </c>
-      <c r="C359" s="6"/>
-      <c r="D359" s="6"/>
-      <c r="E359" s="6"/>
-    </row>
-    <row r="361" spans="1:5">
-      <c r="B361" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C361" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D361" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E361" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="362" spans="1:5">
-      <c r="B362" s="8">
-        <v>1</v>
-      </c>
-      <c r="C362" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="D362" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="E362" s="8" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="363" spans="1:5">
-      <c r="B363" s="8">
-        <v>2</v>
-      </c>
-      <c r="C363" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="D363" s="8" t="s">
-        <v>400</v>
-      </c>
-      <c r="E363" s="8" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="364" spans="1:5">
       <c r="B364" s="8">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C364" s="8" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D364" s="8" t="s">
-        <v>397</v>
+        <v>49</v>
       </c>
       <c r="E364" s="8" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="365" spans="1:5">
-      <c r="B365" s="8">
-        <v>4</v>
-      </c>
-      <c r="C365" s="8" t="s">
-        <v>404</v>
-      </c>
-      <c r="D365" s="8" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="367" spans="1:5">
+      <c r="A367" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B367" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="E365" s="8" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="366" spans="1:5">
-      <c r="B366" s="8">
-        <v>5</v>
-      </c>
-      <c r="C366" s="8" t="s">
-        <v>406</v>
-      </c>
-      <c r="D366" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="E366" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="367" spans="1:5">
-      <c r="B367" s="8">
-        <v>6</v>
-      </c>
-      <c r="C367" s="8" t="s">
-        <v>409</v>
-      </c>
-      <c r="D367" s="8" t="s">
-        <v>410</v>
-      </c>
-      <c r="E367" s="8" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="370" spans="1:5">
-      <c r="A370" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B370" s="5" t="s">
-        <v>422</v>
-      </c>
-      <c r="C370" s="5"/>
-      <c r="D370" s="5"/>
-      <c r="E370" s="5"/>
+      <c r="C367" s="5"/>
+      <c r="D367" s="5"/>
+      <c r="E367" s="5"/>
+    </row>
+    <row r="368" spans="1:5">
+      <c r="A368" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B368" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C368" s="6"/>
+      <c r="D368" s="6"/>
+      <c r="E368" s="6"/>
+    </row>
+    <row r="369" spans="1:5">
+      <c r="A369" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B369" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="C369" s="6"/>
+      <c r="D369" s="6"/>
+      <c r="E369" s="6"/>
     </row>
     <row r="371" spans="1:5">
-      <c r="A371" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B371" s="6" t="s">
-        <v>351</v>
-      </c>
-      <c r="C371" s="6"/>
-      <c r="D371" s="6"/>
-      <c r="E371" s="6"/>
+      <c r="B371" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C371" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D371" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E371" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="372" spans="1:5">
       <c r="B372" s="8">
-        <v>0</v>
-      </c>
-      <c r="C372" s="8"/>
+        <v>1</v>
+      </c>
+      <c r="C372" s="8" t="s">
+        <v>402</v>
+      </c>
       <c r="D372" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="E372" s="8"/>
+        <v>363</v>
+      </c>
+      <c r="E372" s="8" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="373" spans="1:5">
+      <c r="B373" s="8">
+        <v>2</v>
+      </c>
+      <c r="C373" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="D373" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="E373" s="8" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="374" spans="1:5">
+      <c r="B374" s="8">
+        <v>3</v>
+      </c>
+      <c r="C374" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="D374" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="E374" s="8" t="s">
+        <v>408</v>
+      </c>
     </row>
     <row r="375" spans="1:5">
-      <c r="A375" s="4" t="s">
+      <c r="B375" s="8">
+        <v>4</v>
+      </c>
+      <c r="C375" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="D375" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="E375" s="8" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="376" spans="1:5">
+      <c r="B376" s="8">
+        <v>5</v>
+      </c>
+      <c r="C376" s="8" t="s">
+        <v>411</v>
+      </c>
+      <c r="D376" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="E376" s="8" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="377" spans="1:5">
+      <c r="B377" s="8">
+        <v>6</v>
+      </c>
+      <c r="C377" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="D377" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="E377" s="8" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="380" spans="1:5">
+      <c r="A380" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B375" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="C375" s="5"/>
-      <c r="D375" s="5"/>
-      <c r="E375" s="5"/>
-    </row>
-    <row r="376" spans="1:5">
-      <c r="A376" s="4" t="s">
+      <c r="B380" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="C380" s="5"/>
+      <c r="D380" s="5"/>
+      <c r="E380" s="5"/>
+    </row>
+    <row r="381" spans="1:5">
+      <c r="A381" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B376" s="6" t="s">
+      <c r="B381" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C376" s="6"/>
-      <c r="D376" s="6"/>
-      <c r="E376" s="6"/>
-    </row>
-    <row r="378" spans="1:5">
-      <c r="B378" s="7" t="s">
+      <c r="C381" s="6"/>
+      <c r="D381" s="6"/>
+      <c r="E381" s="6"/>
+    </row>
+    <row r="382" spans="1:5">
+      <c r="A382" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B382" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="C382" s="6"/>
+      <c r="D382" s="6"/>
+      <c r="E382" s="6"/>
+    </row>
+    <row r="384" spans="1:5">
+      <c r="B384" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C378" s="7" t="s">
+      <c r="C384" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D378" s="7" t="s">
+      <c r="D384" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E378" s="7" t="s">
+      <c r="E384" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="379" spans="1:5">
-      <c r="B379" s="8">
+    <row r="385" spans="1:5">
+      <c r="B385" s="8">
         <v>1</v>
       </c>
-      <c r="C379" s="8" t="s">
-        <v>424</v>
-      </c>
-      <c r="D379" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E379" s="8"/>
-    </row>
-    <row r="380" spans="1:5">
-      <c r="B380" s="8">
+      <c r="C385" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="D385" s="8" t="s">
+        <v>430</v>
+      </c>
+      <c r="E385" s="8" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="386" spans="1:5">
+      <c r="B386" s="8">
         <v>2</v>
       </c>
-      <c r="C380" s="8" t="s">
-        <v>425</v>
-      </c>
-      <c r="D380" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="E380" s="8"/>
-    </row>
-    <row r="381" spans="1:5">
-      <c r="B381" s="8">
-        <v>3</v>
-      </c>
-      <c r="C381" s="8" t="s">
-        <v>426</v>
-      </c>
-      <c r="D381" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="E381" s="8"/>
-    </row>
-    <row r="382" spans="1:5">
-      <c r="B382" s="8">
-        <v>4</v>
-      </c>
-      <c r="C382" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="D382" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="E382" s="8"/>
-    </row>
-    <row r="385" spans="1:5">
-      <c r="A385" s="4" t="s">
+      <c r="C386" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="D386" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="E386" s="8" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="389" spans="1:5">
+      <c r="A389" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B385" s="5" t="s">
-        <v>428</v>
-      </c>
-      <c r="C385" s="5"/>
-      <c r="D385" s="5"/>
-      <c r="E385" s="5"/>
-    </row>
-    <row r="386" spans="1:5">
-      <c r="A386" s="4" t="s">
+      <c r="B389" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C389" s="5"/>
+      <c r="D389" s="5"/>
+      <c r="E389" s="5"/>
+    </row>
+    <row r="390" spans="1:5">
+      <c r="A390" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B386" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C386" s="6"/>
-      <c r="D386" s="6"/>
-      <c r="E386" s="6"/>
-    </row>
-    <row r="387" spans="1:5">
-      <c r="A387" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B387" s="6" t="s">
-        <v>429</v>
-      </c>
-      <c r="C387" s="6"/>
-      <c r="D387" s="6"/>
-      <c r="E387" s="6"/>
-    </row>
-    <row r="389" spans="1:5">
-      <c r="B389" s="7" t="s">
+      <c r="B390" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C390" s="6"/>
+      <c r="D390" s="6"/>
+      <c r="E390" s="6"/>
+    </row>
+    <row r="392" spans="1:5">
+      <c r="B392" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C389" s="7" t="s">
+      <c r="C392" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D389" s="7" t="s">
+      <c r="D392" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E389" s="7" t="s">
+      <c r="E392" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="390" spans="1:5">
-      <c r="B390" s="8">
-        <v>1</v>
-      </c>
-      <c r="C390" s="8" t="s">
-        <v>430</v>
-      </c>
-      <c r="D390" s="8" t="s">
-        <v>431</v>
-      </c>
-      <c r="E390" s="8" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="391" spans="1:5">
-      <c r="B391" s="8">
-        <v>2</v>
-      </c>
-      <c r="C391" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="D391" s="8" t="s">
-        <v>434</v>
-      </c>
-      <c r="E391" s="8" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="394" spans="1:5">
-      <c r="A394" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B394" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="C394" s="5"/>
-      <c r="D394" s="5"/>
-      <c r="E394" s="5"/>
     </row>
     <row r="395" spans="1:5">
       <c r="A395" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B395" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C395" s="5"/>
+      <c r="D395" s="5"/>
+      <c r="E395" s="5"/>
+    </row>
+    <row r="396" spans="1:5">
+      <c r="A396" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B395" s="6" t="s">
+      <c r="B396" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C395" s="6"/>
-      <c r="D395" s="6"/>
-      <c r="E395" s="6"/>
-    </row>
-    <row r="397" spans="1:5">
-      <c r="B397" s="7" t="s">
+      <c r="C396" s="6"/>
+      <c r="D396" s="6"/>
+      <c r="E396" s="6"/>
+    </row>
+    <row r="398" spans="1:5">
+      <c r="B398" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C397" s="7" t="s">
+      <c r="C398" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D397" s="7" t="s">
+      <c r="D398" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E397" s="7" t="s">
+      <c r="E398" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="400" spans="1:5">
-      <c r="A400" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B400" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C400" s="5"/>
-      <c r="D400" s="5"/>
-      <c r="E400" s="5"/>
     </row>
     <row r="401" spans="1:5">
       <c r="A401" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B401" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C401" s="5"/>
+      <c r="D401" s="5"/>
+      <c r="E401" s="5"/>
+    </row>
+    <row r="402" spans="1:5">
+      <c r="A402" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B401" s="6" t="s">
+      <c r="B402" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C401" s="6"/>
-      <c r="D401" s="6"/>
-      <c r="E401" s="6"/>
-    </row>
-    <row r="403" spans="1:5">
-      <c r="B403" s="7" t="s">
+      <c r="C402" s="6"/>
+      <c r="D402" s="6"/>
+      <c r="E402" s="6"/>
+    </row>
+    <row r="404" spans="1:5">
+      <c r="B404" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C403" s="7" t="s">
+      <c r="C404" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D403" s="7" t="s">
+      <c r="D404" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E403" s="7" t="s">
+      <c r="E404" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="406" spans="1:5">
-      <c r="A406" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B406" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C406" s="5"/>
-      <c r="D406" s="5"/>
-      <c r="E406" s="5"/>
     </row>
     <row r="407" spans="1:5">
       <c r="A407" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B407" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="C407" s="5"/>
+      <c r="D407" s="5"/>
+      <c r="E407" s="5"/>
+    </row>
+    <row r="408" spans="1:5">
+      <c r="A408" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B407" s="6" t="s">
+      <c r="B408" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C407" s="6"/>
-      <c r="D407" s="6"/>
-      <c r="E407" s="6"/>
-    </row>
-    <row r="409" spans="1:5">
-      <c r="B409" s="7" t="s">
+      <c r="C408" s="6"/>
+      <c r="D408" s="6"/>
+      <c r="E408" s="6"/>
+    </row>
+    <row r="410" spans="1:5">
+      <c r="B410" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C409" s="7" t="s">
+      <c r="C410" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D409" s="7" t="s">
+      <c r="D410" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E409" s="7" t="s">
+      <c r="E410" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="412" spans="1:5">
-      <c r="A412" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B412" s="5" t="s">
-        <v>460</v>
-      </c>
-      <c r="C412" s="5"/>
-      <c r="D412" s="5"/>
-      <c r="E412" s="5"/>
     </row>
     <row r="413" spans="1:5">
       <c r="A413" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B413" s="5" t="s">
+        <v>460</v>
+      </c>
+      <c r="C413" s="5"/>
+      <c r="D413" s="5"/>
+      <c r="E413" s="5"/>
+    </row>
+    <row r="414" spans="1:5">
+      <c r="A414" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B413" s="6" t="s">
+      <c r="B414" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C413" s="6"/>
-      <c r="D413" s="6"/>
-      <c r="E413" s="6"/>
-    </row>
-    <row r="415" spans="1:5">
-      <c r="B415" s="7" t="s">
+      <c r="C414" s="6"/>
+      <c r="D414" s="6"/>
+      <c r="E414" s="6"/>
+    </row>
+    <row r="416" spans="1:5">
+      <c r="B416" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C415" s="7" t="s">
+      <c r="C416" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D415" s="7" t="s">
+      <c r="D416" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E415" s="7" t="s">
+      <c r="E416" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="418" spans="1:5">
-      <c r="A418" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B418" s="5" t="s">
-        <v>461</v>
-      </c>
-      <c r="C418" s="5"/>
-      <c r="D418" s="5"/>
-      <c r="E418" s="5"/>
     </row>
     <row r="419" spans="1:5">
       <c r="A419" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B419" s="5" t="s">
+        <v>461</v>
+      </c>
+      <c r="C419" s="5"/>
+      <c r="D419" s="5"/>
+      <c r="E419" s="5"/>
+    </row>
+    <row r="420" spans="1:5">
+      <c r="A420" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B419" s="6" t="s">
+      <c r="B420" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C419" s="6"/>
-      <c r="D419" s="6"/>
-      <c r="E419" s="6"/>
-    </row>
-    <row r="421" spans="1:5">
-      <c r="B421" s="7" t="s">
+      <c r="C420" s="6"/>
+      <c r="D420" s="6"/>
+      <c r="E420" s="6"/>
+    </row>
+    <row r="422" spans="1:5">
+      <c r="B422" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C421" s="7" t="s">
+      <c r="C422" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D421" s="7" t="s">
+      <c r="D422" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E421" s="7" t="s">
+      <c r="E422" s="7" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="424" spans="1:5">
-      <c r="A424" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B424" s="5" t="s">
-        <v>462</v>
-      </c>
-      <c r="C424" s="5"/>
-      <c r="D424" s="5"/>
-      <c r="E424" s="5"/>
-    </row>
-    <row r="425" spans="1:5">
-      <c r="A425" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B425" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C425" s="6"/>
-      <c r="D425" s="6"/>
-      <c r="E425" s="6"/>
-    </row>
-    <row r="427" spans="1:5">
-      <c r="B427" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C427" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D427" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E427" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="104">
+  <mergeCells count="106">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B11:E11"/>
@@ -5747,38 +5694,40 @@
     <mergeCell ref="B310:E310"/>
     <mergeCell ref="B315:E315"/>
     <mergeCell ref="B316:E316"/>
-    <mergeCell ref="B324:E324"/>
-    <mergeCell ref="B325:E325"/>
-    <mergeCell ref="B333:E333"/>
+    <mergeCell ref="B317:E317"/>
+    <mergeCell ref="B320:E320"/>
+    <mergeCell ref="B321:E321"/>
+    <mergeCell ref="B329:E329"/>
+    <mergeCell ref="B330:E330"/>
+    <mergeCell ref="B331:E331"/>
     <mergeCell ref="B334:E334"/>
-    <mergeCell ref="B338:E338"/>
-    <mergeCell ref="B339:E339"/>
+    <mergeCell ref="B335:E335"/>
     <mergeCell ref="B343:E343"/>
     <mergeCell ref="B344:E344"/>
-    <mergeCell ref="B350:E350"/>
-    <mergeCell ref="B351:E351"/>
-    <mergeCell ref="B357:E357"/>
-    <mergeCell ref="B358:E358"/>
-    <mergeCell ref="B359:E359"/>
-    <mergeCell ref="B370:E370"/>
-    <mergeCell ref="B371:E371"/>
-    <mergeCell ref="B375:E375"/>
-    <mergeCell ref="B376:E376"/>
-    <mergeCell ref="B385:E385"/>
-    <mergeCell ref="B386:E386"/>
-    <mergeCell ref="B387:E387"/>
-    <mergeCell ref="B394:E394"/>
+    <mergeCell ref="B348:E348"/>
+    <mergeCell ref="B349:E349"/>
+    <mergeCell ref="B353:E353"/>
+    <mergeCell ref="B354:E354"/>
+    <mergeCell ref="B360:E360"/>
+    <mergeCell ref="B361:E361"/>
+    <mergeCell ref="B367:E367"/>
+    <mergeCell ref="B368:E368"/>
+    <mergeCell ref="B369:E369"/>
+    <mergeCell ref="B380:E380"/>
+    <mergeCell ref="B381:E381"/>
+    <mergeCell ref="B382:E382"/>
+    <mergeCell ref="B389:E389"/>
+    <mergeCell ref="B390:E390"/>
     <mergeCell ref="B395:E395"/>
-    <mergeCell ref="B400:E400"/>
+    <mergeCell ref="B396:E396"/>
     <mergeCell ref="B401:E401"/>
-    <mergeCell ref="B406:E406"/>
+    <mergeCell ref="B402:E402"/>
     <mergeCell ref="B407:E407"/>
-    <mergeCell ref="B412:E412"/>
+    <mergeCell ref="B408:E408"/>
     <mergeCell ref="B413:E413"/>
-    <mergeCell ref="B418:E418"/>
+    <mergeCell ref="B414:E414"/>
     <mergeCell ref="B419:E419"/>
-    <mergeCell ref="B424:E424"/>
-    <mergeCell ref="B425:E425"/>
+    <mergeCell ref="B420:E420"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6635,7 +6584,7 @@
         <v>55</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
@@ -6645,7 +6594,7 @@
         <v>92</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="C112" s="6"/>
       <c r="D112" s="6"/>
@@ -6666,10 +6615,10 @@
         <v>2048</v>
       </c>
       <c r="C115" s="8" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -6677,10 +6626,10 @@
         <v>2054</v>
       </c>
       <c r="C116" s="8" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -6688,10 +6637,10 @@
         <v>34525</v>
       </c>
       <c r="C117" s="8" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -6699,10 +6648,10 @@
         <v>34887</v>
       </c>
       <c r="C118" s="8" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -6710,7 +6659,7 @@
         <v>55</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C120" s="5"/>
       <c r="D120" s="5"/>
@@ -6720,7 +6669,7 @@
         <v>92</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C121" s="6"/>
       <c r="D121" s="6"/>
@@ -6741,10 +6690,10 @@
         <v>1</v>
       </c>
       <c r="C124" s="8" t="s">
+        <v>437</v>
+      </c>
+      <c r="D124" s="8" t="s">
         <v>438</v>
-      </c>
-      <c r="D124" s="8" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -6752,10 +6701,10 @@
         <v>6</v>
       </c>
       <c r="C125" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="D125" s="8" t="s">
         <v>440</v>
-      </c>
-      <c r="D125" s="8" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -6763,10 +6712,10 @@
         <v>17</v>
       </c>
       <c r="C126" s="8" t="s">
+        <v>441</v>
+      </c>
+      <c r="D126" s="8" t="s">
         <v>442</v>
-      </c>
-      <c r="D126" s="8" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -6774,7 +6723,7 @@
         <v>55</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C128" s="5"/>
       <c r="D128" s="5"/>
@@ -6784,7 +6733,7 @@
         <v>92</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C129" s="6"/>
       <c r="D129" s="6"/>
@@ -6805,10 +6754,10 @@
         <v>20</v>
       </c>
       <c r="C132" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="D132" s="8" t="s">
         <v>446</v>
-      </c>
-      <c r="D132" s="8" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -6816,10 +6765,10 @@
         <v>21</v>
       </c>
       <c r="C133" s="8" t="s">
+        <v>447</v>
+      </c>
+      <c r="D133" s="8" t="s">
         <v>448</v>
-      </c>
-      <c r="D133" s="8" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -6827,10 +6776,10 @@
         <v>22</v>
       </c>
       <c r="C134" s="8" t="s">
+        <v>449</v>
+      </c>
+      <c r="D134" s="8" t="s">
         <v>450</v>
-      </c>
-      <c r="D134" s="8" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -6838,10 +6787,10 @@
         <v>23</v>
       </c>
       <c r="C135" s="8" t="s">
+        <v>451</v>
+      </c>
+      <c r="D135" s="8" t="s">
         <v>452</v>
-      </c>
-      <c r="D135" s="8" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -6849,10 +6798,10 @@
         <v>25</v>
       </c>
       <c r="C136" s="8" t="s">
+        <v>453</v>
+      </c>
+      <c r="D136" s="8" t="s">
         <v>454</v>
-      </c>
-      <c r="D136" s="8" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -6860,10 +6809,10 @@
         <v>80</v>
       </c>
       <c r="C137" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="D137" s="8" t="s">
         <v>456</v>
-      </c>
-      <c r="D137" s="8" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -6871,10 +6820,10 @@
         <v>443</v>
       </c>
       <c r="C138" s="8" t="s">
+        <v>457</v>
+      </c>
+      <c r="D138" s="8" t="s">
         <v>458</v>
-      </c>
-      <c r="D138" s="8" t="s">
-        <v>459</v>
       </c>
     </row>
   </sheetData>

</xml_diff>